<commit_message>
Fix windows file path forward/backslash
</commit_message>
<xml_diff>
--- a/Beagle_en_pages_report.xlsx
+++ b/Beagle_en_pages_report.xlsx
@@ -7,14 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="local assets" r:id="rId5" sheetId="13"/>
-    <sheet name="todos" r:id="rId6" sheetId="15"/>
-    <sheet name="page map" r:id="rId7" sheetId="16"/>
+    <sheet name="todos" r:id="rId6" sheetId="21"/>
+    <sheet name="page map" r:id="rId7" sheetId="22"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4126" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6334" uniqueCount="1190">
   <si>
     <t>asset</t>
   </si>
@@ -3594,13 +3594,43 @@
     <numFmt numFmtId="164" formatCode="yyyy-MM-dd"/>
     <numFmt numFmtId="165" formatCode="###0.0"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="24">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -3718,7 +3748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -3771,6 +3801,24 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -5483,7 +5531,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -5494,15 +5542,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="43.76953125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="89.5703125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="43.6875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="89.2109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="48">
+      <c r="A1" t="s" s="66">
         <v>528</v>
       </c>
-      <c r="B1" t="s" s="48">
+      <c r="B1" t="s" s="66">
         <v>529</v>
       </c>
     </row>
@@ -5519,7 +5567,7 @@
         <v>532</v>
       </c>
       <c r="B3" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="4">
@@ -5527,7 +5575,7 @@
         <v>532</v>
       </c>
       <c r="B4" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="5">
@@ -5535,7 +5583,7 @@
         <v>532</v>
       </c>
       <c r="B5" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="6">
@@ -5572,18 +5620,18 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="B10" t="s">
-        <v>539</v>
+        <v>543</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B11" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="12">
@@ -5596,18 +5644,18 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B13" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="B14" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="15">
@@ -5615,7 +5663,7 @@
         <v>549</v>
       </c>
       <c r="B15" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
     </row>
     <row r="16">
@@ -5623,23 +5671,23 @@
         <v>549</v>
       </c>
       <c r="B16" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B17" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="B18" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="19">
@@ -5735,9 +5783,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B341"/>
+  <dimension ref="A1:B339"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -5746,15 +5794,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="103.0234375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="101.16796875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="103.17578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="101.25" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="51">
+      <c r="A1" t="s" s="69">
         <v>422</v>
       </c>
-      <c r="B1" t="s" s="51">
+      <c r="B1" t="s" s="69">
         <v>423</v>
       </c>
     </row>
@@ -5792,18 +5840,18 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="B6" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="B7" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="8">
@@ -5888,26 +5936,26 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="B18" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="B19" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B20" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="21">
@@ -6064,18 +6112,18 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>477</v>
+        <v>634</v>
       </c>
       <c r="B40" t="s">
-        <v>503</v>
+        <v>635</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>634</v>
+        <v>477</v>
       </c>
       <c r="B41" t="s">
-        <v>635</v>
+        <v>503</v>
       </c>
     </row>
     <row r="42">
@@ -6184,18 +6232,18 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>658</v>
+        <v>660</v>
       </c>
       <c r="B55" t="s">
-        <v>659</v>
+        <v>661</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B56" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="57">
@@ -6232,10 +6280,10 @@
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>670</v>
+        <v>492</v>
       </c>
       <c r="B61" t="s">
-        <v>671</v>
+        <v>518</v>
       </c>
     </row>
     <row r="62">
@@ -6248,10 +6296,10 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>492</v>
+        <v>670</v>
       </c>
       <c r="B63" t="s">
-        <v>518</v>
+        <v>671</v>
       </c>
     </row>
     <row r="64">
@@ -6288,18 +6336,18 @@
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="B68" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B69" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="70">
@@ -6320,18 +6368,18 @@
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="B72" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B73" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="74">
@@ -6360,18 +6408,18 @@
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="B77" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="B78" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
     </row>
     <row r="79">
@@ -6440,18 +6488,18 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="B87" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="B88" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
     </row>
     <row r="89">
@@ -6504,18 +6552,18 @@
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="B95" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="B96" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
     </row>
     <row r="97">
@@ -6544,18 +6592,18 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="B100" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="B101" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="102">
@@ -6624,26 +6672,26 @@
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="B110" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="B111" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="B112" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="113">
@@ -6656,18 +6704,18 @@
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="B114" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B115" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="116">
@@ -6728,42 +6776,42 @@
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>784</v>
+        <v>790</v>
       </c>
       <c r="B123" t="s">
-        <v>785</v>
+        <v>791</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>786</v>
+        <v>792</v>
       </c>
       <c r="B124" t="s">
-        <v>787</v>
+        <v>793</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="B125" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="B126" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="s">
-        <v>792</v>
+        <v>784</v>
       </c>
       <c r="B127" t="s">
-        <v>793</v>
+        <v>785</v>
       </c>
     </row>
     <row r="128">
@@ -6888,18 +6936,18 @@
     </row>
     <row r="143">
       <c r="A143" t="s">
-        <v>490</v>
+        <v>820</v>
       </c>
       <c r="B143" t="s">
-        <v>516</v>
+        <v>821</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="s">
-        <v>820</v>
+        <v>490</v>
       </c>
       <c r="B144" t="s">
-        <v>821</v>
+        <v>516</v>
       </c>
     </row>
     <row r="145">
@@ -6912,10 +6960,10 @@
     </row>
     <row r="146">
       <c r="A146" t="s">
-        <v>824</v>
+        <v>828</v>
       </c>
       <c r="B146" t="s">
-        <v>825</v>
+        <v>829</v>
       </c>
     </row>
     <row r="147">
@@ -6928,10 +6976,10 @@
     </row>
     <row r="148">
       <c r="A148" t="s">
-        <v>828</v>
+        <v>824</v>
       </c>
       <c r="B148" t="s">
-        <v>829</v>
+        <v>825</v>
       </c>
     </row>
     <row r="149">
@@ -7024,34 +7072,34 @@
     </row>
     <row r="160">
       <c r="A160" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="B160" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="B161" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="B162" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
       <c r="B163" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="164">
@@ -7168,18 +7216,18 @@
     </row>
     <row r="178">
       <c r="A178" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="B178" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="B179" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="180">
@@ -7192,10 +7240,10 @@
     </row>
     <row r="181">
       <c r="A181" t="s">
-        <v>886</v>
+        <v>890</v>
       </c>
       <c r="B181" t="s">
-        <v>887</v>
+        <v>891</v>
       </c>
     </row>
     <row r="182">
@@ -7208,10 +7256,10 @@
     </row>
     <row r="183">
       <c r="A183" t="s">
-        <v>890</v>
+        <v>886</v>
       </c>
       <c r="B183" t="s">
-        <v>891</v>
+        <v>887</v>
       </c>
     </row>
     <row r="184">
@@ -7312,18 +7360,18 @@
     </row>
     <row r="196">
       <c r="A196" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="B196" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="B197" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="198">
@@ -7448,18 +7496,18 @@
     </row>
     <row r="213">
       <c r="A213" t="s">
-        <v>948</v>
+        <v>491</v>
       </c>
       <c r="B213" t="s">
-        <v>949</v>
+        <v>517</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="s">
-        <v>491</v>
+        <v>948</v>
       </c>
       <c r="B214" t="s">
-        <v>517</v>
+        <v>949</v>
       </c>
     </row>
     <row r="215">
@@ -7480,18 +7528,18 @@
     </row>
     <row r="217">
       <c r="A217" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="B217" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="B218" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
     </row>
     <row r="219">
@@ -7536,18 +7584,18 @@
     </row>
     <row r="224">
       <c r="A224" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="B224" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="B225" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
     </row>
     <row r="226">
@@ -7568,18 +7616,18 @@
     </row>
     <row r="228">
       <c r="A228" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="B228" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="B229" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
     </row>
     <row r="230">
@@ -7600,26 +7648,26 @@
     </row>
     <row r="232">
       <c r="A232" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
       <c r="B232" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="B233" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="B234" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
     </row>
     <row r="235">
@@ -7648,34 +7696,34 @@
     </row>
     <row r="238">
       <c r="A238" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="B238" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="B239" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="B240" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="s">
-        <v>1002</v>
+        <v>1006</v>
       </c>
       <c r="B241" t="s">
-        <v>1003</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="242">
@@ -7688,74 +7736,74 @@
     </row>
     <row r="243">
       <c r="A243" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B243" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="B244" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="B245" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="B246" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="247">
       <c r="A247" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="B247" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
     </row>
     <row r="248">
       <c r="A248" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="B248" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="B249" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="B250" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="s">
-        <v>1022</v>
+        <v>1026</v>
       </c>
       <c r="B251" t="s">
-        <v>1023</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="252">
@@ -7768,26 +7816,26 @@
     </row>
     <row r="253">
       <c r="A253" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="B253" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
     </row>
     <row r="254">
       <c r="A254" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="B254" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="s">
-        <v>1030</v>
+        <v>1034</v>
       </c>
       <c r="B255" t="s">
-        <v>1031</v>
+        <v>1035</v>
       </c>
     </row>
     <row r="256">
@@ -7800,10 +7848,10 @@
     </row>
     <row r="257">
       <c r="A257" t="s">
-        <v>1034</v>
+        <v>1038</v>
       </c>
       <c r="B257" t="s">
-        <v>1035</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="258">
@@ -7816,50 +7864,50 @@
     </row>
     <row r="259">
       <c r="A259" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="B259" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="B260" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="B261" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="B262" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s">
-        <v>1046</v>
+        <v>495</v>
       </c>
       <c r="B263" t="s">
-        <v>1047</v>
+        <v>521</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s">
-        <v>495</v>
+        <v>1050</v>
       </c>
       <c r="B264" t="s">
-        <v>521</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="265">
@@ -7872,34 +7920,34 @@
     </row>
     <row r="266">
       <c r="A266" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="B266" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="B267" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="B268" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c r="B269" t="s">
-        <v>1057</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="270">
@@ -7912,154 +7960,154 @@
     </row>
     <row r="271">
       <c r="A271" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="B271" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
       <c r="B272" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="B273" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="B274" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
       <c r="B275" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="B276" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="B277" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
       <c r="B278" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="B279" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="B280" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
       <c r="B281" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="B282" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="B283" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
       <c r="B284" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="B285" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s">
-        <v>1090</v>
+        <v>476</v>
       </c>
       <c r="B286" t="s">
-        <v>1091</v>
+        <v>502</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="s">
-        <v>476</v>
+        <v>1092</v>
       </c>
       <c r="B287" t="s">
-        <v>502</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="B288" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="s">
-        <v>1094</v>
+        <v>479</v>
       </c>
       <c r="B289" t="s">
-        <v>1095</v>
+        <v>505</v>
       </c>
     </row>
     <row r="290">
@@ -8072,409 +8120,393 @@
     </row>
     <row r="291">
       <c r="A291" t="s">
-        <v>479</v>
+        <v>1096</v>
       </c>
       <c r="B291" t="s">
-        <v>505</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="292">
       <c r="A292" t="s">
-        <v>1096</v>
+        <v>1100</v>
       </c>
       <c r="B292" t="s">
-        <v>1097</v>
+        <v>1101</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="s">
-        <v>1098</v>
+        <v>480</v>
       </c>
       <c r="B293" t="s">
-        <v>1099</v>
+        <v>506</v>
       </c>
     </row>
     <row r="294">
       <c r="A294" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="B294" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="s">
-        <v>480</v>
+        <v>1104</v>
       </c>
       <c r="B295" t="s">
-        <v>506</v>
+        <v>1105</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="s">
-        <v>1102</v>
+        <v>1106</v>
       </c>
       <c r="B296" t="s">
-        <v>1103</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="s">
-        <v>1104</v>
+        <v>1108</v>
       </c>
       <c r="B297" t="s">
-        <v>1105</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="s">
-        <v>1106</v>
+        <v>1110</v>
       </c>
       <c r="B298" t="s">
-        <v>1107</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="s">
-        <v>1108</v>
+        <v>1112</v>
       </c>
       <c r="B299" t="s">
-        <v>1109</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="s">
-        <v>1110</v>
+        <v>1114</v>
       </c>
       <c r="B300" t="s">
-        <v>1111</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="s">
-        <v>1112</v>
+        <v>1116</v>
       </c>
       <c r="B301" t="s">
-        <v>1113</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="302">
       <c r="A302" t="s">
-        <v>1114</v>
+        <v>1118</v>
       </c>
       <c r="B302" t="s">
-        <v>1115</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" t="s">
-        <v>1116</v>
+        <v>1120</v>
       </c>
       <c r="B303" t="s">
-        <v>1117</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="s">
-        <v>1118</v>
+        <v>1122</v>
       </c>
       <c r="B304" t="s">
-        <v>1119</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="s">
-        <v>1120</v>
+        <v>1124</v>
       </c>
       <c r="B305" t="s">
-        <v>1121</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="s">
-        <v>1122</v>
+        <v>487</v>
       </c>
       <c r="B306" t="s">
-        <v>1123</v>
+        <v>513</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="B307" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="s">
-        <v>487</v>
+        <v>1128</v>
       </c>
       <c r="B308" t="s">
-        <v>513</v>
+        <v>1129</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="s">
-        <v>1126</v>
+        <v>1130</v>
       </c>
       <c r="B309" t="s">
-        <v>1127</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="s">
-        <v>1128</v>
+        <v>1132</v>
       </c>
       <c r="B310" t="s">
-        <v>1129</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" t="s">
-        <v>1130</v>
+        <v>1134</v>
       </c>
       <c r="B311" t="s">
-        <v>1131</v>
+        <v>1135</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="s">
-        <v>1132</v>
+        <v>1136</v>
       </c>
       <c r="B312" t="s">
-        <v>1133</v>
+        <v>1137</v>
       </c>
     </row>
     <row r="313">
       <c r="A313" t="s">
-        <v>1134</v>
+        <v>1138</v>
       </c>
       <c r="B313" t="s">
-        <v>1135</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="s">
-        <v>1136</v>
+        <v>1142</v>
       </c>
       <c r="B314" t="s">
-        <v>1137</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="B315" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" t="s">
-        <v>1140</v>
+        <v>1144</v>
       </c>
       <c r="B316" t="s">
-        <v>1141</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="317">
       <c r="A317" t="s">
-        <v>1142</v>
+        <v>1146</v>
       </c>
       <c r="B317" t="s">
-        <v>1143</v>
+        <v>1147</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="s">
-        <v>1144</v>
+        <v>1148</v>
       </c>
       <c r="B318" t="s">
-        <v>1145</v>
+        <v>1149</v>
       </c>
     </row>
     <row r="319">
       <c r="A319" t="s">
-        <v>1146</v>
+        <v>1150</v>
       </c>
       <c r="B319" t="s">
-        <v>1147</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="s">
-        <v>1148</v>
+        <v>1152</v>
       </c>
       <c r="B320" t="s">
-        <v>1149</v>
+        <v>1153</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="s">
-        <v>1150</v>
+        <v>1154</v>
       </c>
       <c r="B321" t="s">
-        <v>1151</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="s">
-        <v>1152</v>
+        <v>1156</v>
       </c>
       <c r="B322" t="s">
-        <v>1153</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="323">
       <c r="A323" t="s">
-        <v>1154</v>
+        <v>1158</v>
       </c>
       <c r="B323" t="s">
-        <v>1155</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="324">
       <c r="A324" t="s">
-        <v>1156</v>
+        <v>1160</v>
       </c>
       <c r="B324" t="s">
-        <v>1157</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="s">
-        <v>1158</v>
+        <v>1162</v>
       </c>
       <c r="B325" t="s">
-        <v>1159</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" t="s">
-        <v>1160</v>
+        <v>1164</v>
       </c>
       <c r="B326" t="s">
-        <v>1161</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="s">
-        <v>1162</v>
+        <v>1166</v>
       </c>
       <c r="B327" t="s">
-        <v>1163</v>
+        <v>1167</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="s">
-        <v>1164</v>
+        <v>1170</v>
       </c>
       <c r="B328" t="s">
-        <v>1165</v>
+        <v>1171</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" t="s">
-        <v>1166</v>
+        <v>1168</v>
       </c>
       <c r="B329" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="s">
-        <v>1168</v>
+        <v>1172</v>
       </c>
       <c r="B330" t="s">
-        <v>1169</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="s">
-        <v>1170</v>
+        <v>1174</v>
       </c>
       <c r="B331" t="s">
-        <v>1171</v>
+        <v>1175</v>
       </c>
     </row>
     <row r="332">
       <c r="A332" t="s">
-        <v>1172</v>
+        <v>1176</v>
       </c>
       <c r="B332" t="s">
-        <v>1173</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="s">
-        <v>1174</v>
+        <v>1178</v>
       </c>
       <c r="B333" t="s">
-        <v>1175</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="s">
-        <v>1176</v>
+        <v>1180</v>
       </c>
       <c r="B334" t="s">
-        <v>1177</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="s">
-        <v>1178</v>
+        <v>1184</v>
       </c>
       <c r="B335" t="s">
-        <v>1179</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="s">
-        <v>1180</v>
+        <v>1182</v>
       </c>
       <c r="B336" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="s">
-        <v>1182</v>
+        <v>501</v>
       </c>
       <c r="B337" t="s">
-        <v>1183</v>
+        <v>527</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="B338" t="s">
-        <v>1185</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="s">
-        <v>1186</v>
+        <v>1188</v>
       </c>
       <c r="B339" t="s">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="340">
-      <c r="A340" t="s">
-        <v>501</v>
-      </c>
-      <c r="B340" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="341">
-      <c r="A341" t="s">
-        <v>1188</v>
-      </c>
-      <c r="B341" t="s">
         <v>1189</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix filter Fragment entry of filter
</commit_message>
<xml_diff>
--- a/Beagle_en_pages_report.xlsx
+++ b/Beagle_en_pages_report.xlsx
@@ -7,14 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="local assets" r:id="rId5" sheetId="13"/>
-    <sheet name="todos" r:id="rId6" sheetId="21"/>
-    <sheet name="page map" r:id="rId7" sheetId="22"/>
+    <sheet name="todos" r:id="rId6" sheetId="25"/>
+    <sheet name="page map" r:id="rId7" sheetId="26"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6334" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7860" uniqueCount="1190">
   <si>
     <t>asset</t>
   </si>
@@ -3594,13 +3594,38 @@
     <numFmt numFmtId="164" formatCode="yyyy-MM-dd"/>
     <numFmt numFmtId="165" formatCode="###0.0"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="29">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -3748,7 +3773,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -3819,6 +3844,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="23" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -5531,7 +5571,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -5547,10 +5587,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="66">
+      <c r="A1" t="s" s="81">
         <v>528</v>
       </c>
-      <c r="B1" t="s" s="66">
+      <c r="B1" t="s" s="81">
         <v>529</v>
       </c>
     </row>
@@ -5783,7 +5823,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B339"/>
   <sheetViews>
@@ -5799,10 +5839,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="69">
+      <c r="A1" t="s" s="84">
         <v>422</v>
       </c>
-      <c r="B1" t="s" s="69">
+      <c r="B1" t="s" s="84">
         <v>423</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added OS detection for windows
</commit_message>
<xml_diff>
--- a/Beagle_en_pages_report.xlsx
+++ b/Beagle_en_pages_report.xlsx
@@ -7,14 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="local assets" r:id="rId5" sheetId="13"/>
-    <sheet name="todos" r:id="rId6" sheetId="25"/>
-    <sheet name="page map" r:id="rId7" sheetId="26"/>
+    <sheet name="todos" r:id="rId6" sheetId="39"/>
+    <sheet name="page map" r:id="rId7" sheetId="40"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7860" uniqueCount="1190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13012" uniqueCount="1190">
   <si>
     <t>asset</t>
   </si>
@@ -3594,13 +3594,83 @@
     <numFmt numFmtId="164" formatCode="yyyy-MM-dd"/>
     <numFmt numFmtId="165" formatCode="###0.0"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="43">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -3773,7 +3843,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -3859,6 +3929,48 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="28" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="30" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="32" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="37" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="40" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="41" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="42" fillId="3" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -5571,7 +5683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -5587,10 +5699,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="81">
+      <c r="A1" t="s" s="123">
         <v>528</v>
       </c>
-      <c r="B1" t="s" s="81">
+      <c r="B1" t="s" s="123">
         <v>529</v>
       </c>
     </row>
@@ -5823,7 +5935,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:B339"/>
   <sheetViews>
@@ -5839,10 +5951,10 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="84">
+      <c r="A1" t="s" s="126">
         <v>422</v>
       </c>
-      <c r="B1" t="s" s="84">
+      <c r="B1" t="s" s="126">
         <v>423</v>
       </c>
     </row>

</xml_diff>